<commit_message>
best working version rn
</commit_message>
<xml_diff>
--- a/card_summary_highlighted.xlsx
+++ b/card_summary_highlighted.xlsx
@@ -113,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -152,12 +152,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -240,366 +234,484 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Matching System</author>
+    <author>Difference Summary</author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <t>Expected: $303.92
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-303.92
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <t>Expected: $77,821.95
-Found: $77,272.47
+Found in UNMATCHED transactions: $77,272.47
 Difference: $-549.48
-Transactions found: 4
-Reason: No match found after all filters</t>
+Unmatched transactions available: 4
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,410.20
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-1,410.20
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <t>Expected: $2,969.96
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-2,969.96
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F6" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,187.63
-Found: $77,632.71
+Found in UNMATCHED transactions: $77,632.71
 Difference: $76,445.08
-Transactions found: 5
-Reason: No match found after all filters</t>
+Unmatched transactions available: 5
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <t>Expected: $371.77
-Found: $78,166.63
+Found in UNMATCHED transactions: $78,166.63
 Difference: $77,794.86
-Transactions found: 4
-Reason: No match found after all filters</t>
+Unmatched transactions available: 4
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <t>Expected: $315.00
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-315.00
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F8" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,302.32
-Found: $2,771.52
+Found in UNMATCHED transactions: $2,771.52
 Difference: $1,469.20
-Transactions found: 3
-Reason: No match found after all filters</t>
+Unmatched transactions available: 3
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,074.43
-Found: $4,765.35
-Difference: $3,690.92
-Transactions found: 6
-Reason: No match found after all filters</t>
+Found in UNMATCHED transactions: $950.13
+Difference: $-124.30
+Unmatched transactions available: 5
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <t>Expected: $584.20
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-584.20
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F9" authorId="0" shapeId="0">
       <text>
         <t>Expected: $744.67
-Found: $1,625.85
+Found in UNMATCHED transactions: $1,625.85
 Difference: $881.18
-Transactions found: 2
-Reason: No match found after all filters</t>
+Unmatched transactions available: 2
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <t>Expected: $450.00
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-450.00
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="E10" authorId="0" shapeId="0">
       <text>
         <t>Expected: $54.22
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-54.22
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I10" authorId="0" shapeId="0">
       <text>
         <t>Expected: $714.76
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-714.76
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <t>Expected: $77.90
-Found: $797.31
+Found in UNMATCHED transactions: $797.31
 Difference: $719.41
-Transactions found: 2
-Reason: No match found after all filters</t>
+Unmatched transactions available: 2
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0">
+      <text>
+        <t>Expected: $-143.36
+Found in UNMATCHED transactions: $797.31
+Difference: $940.67
+Unmatched transactions available: 2
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0">
+      <text>
+        <t>Expected: $-38.76
+Found in UNMATCHED transactions: $2,512.21
+Difference: $2,550.97
+Unmatched transactions available: 3
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F14" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,964.56
-Found: $1,714.90
+Found in UNMATCHED transactions: $1,714.90
 Difference: $-249.66
-Transactions found: 1
-Reason: No match found after all filters</t>
+Unmatched transactions available: 1
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I14" authorId="0" shapeId="0">
       <text>
         <t>Expected: $84.58
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-84.58
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="J14" authorId="0" shapeId="0">
       <text>
         <t>Expected: $500.00
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-500.00
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="B15" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,009.13
-Found: $2,211.15
-Difference: $1,202.02
-Transactions found: 5
-Reason: No match found after all filters</t>
+Found in UNMATCHED transactions: $1,655.49
+Difference: $646.36
+Unmatched transactions available: 2
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0">
+      <text>
+        <t>Expected: $-291.63
+Found in UNMATCHED transactions: $1,714.90
+Difference: $2,006.53
+Unmatched transactions available: 1
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I16" authorId="0" shapeId="0">
       <text>
         <t>Expected: $293.25
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-293.25
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F18" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,439.19
-Found: $1,085.02
+Found in UNMATCHED transactions: $1,085.02
 Difference: $-354.17
-Transactions found: 2
-Reason: No match found after all filters</t>
+Unmatched transactions available: 2
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I18" authorId="0" shapeId="0">
       <text>
         <t>Expected: $60.00
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-60.00
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F20" authorId="0" shapeId="0">
       <text>
         <t>Expected: $513.02
-Found: $1,721.99
+Found in UNMATCHED transactions: $1,721.99
 Difference: $1,208.97
-Transactions found: 4
-Reason: No match found after all filters</t>
+Unmatched transactions available: 4
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F21" authorId="0" shapeId="0">
       <text>
         <t>Expected: $143.88
-Found: $1,032.29
+Found in UNMATCHED transactions: $1,032.29
 Difference: $888.41
-Transactions found: 3
-Reason: No match found after all filters</t>
+Unmatched transactions available: 3
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F22" authorId="0" shapeId="0">
       <text>
         <t>Expected: $410.50
-Found: $1,032.29
+Found in UNMATCHED transactions: $1,032.29
 Difference: $621.79
-Transactions found: 3
-Reason: No match found after all filters</t>
+Unmatched transactions available: 3
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I22" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,155.00
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-1,155.00
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="B24" authorId="0" shapeId="0">
       <text>
         <t>Expected: $15.05
-Found: $1,240.49
-Difference: $1,225.44
-Transactions found: 8
-Reason: No match found after all filters</t>
+Found in UNMATCHED transactions: $-45.87
+Difference: $-60.92
+Unmatched transactions available: 2
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="F24" authorId="0" shapeId="0">
+      <text>
+        <t>Expected: $-136.36
+Found in UNMATCHED transactions: $395.32
+Difference: $531.68
+Unmatched transactions available: 1
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="J24" authorId="0" shapeId="0">
       <text>
         <t>Expected: $4,699.67
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-4,699.67
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="K24" authorId="0" shapeId="0">
+      <text>
+        <t>Expected: $-60.92
+Found in UNMATCHED transactions: $0.00
+Difference: $60.92
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="F25" authorId="0" shapeId="0">
+      <text>
+        <t>Expected: $-341.71
+Found in UNMATCHED transactions: $0.00
+Difference: $341.71
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F26" authorId="0" shapeId="0">
       <text>
         <t>Expected: $23.72
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-23.72
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I26" authorId="0" shapeId="0">
       <text>
         <t>Expected: $10.20
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-10.20
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I27" authorId="0" shapeId="0">
       <text>
         <t>Expected: $33.17
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-33.17
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="F28" authorId="0" shapeId="0">
+      <text>
+        <t>Expected: $-43.17
+Found in UNMATCHED transactions: $0.00
+Difference: $43.17
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I28" authorId="0" shapeId="0">
       <text>
         <t>Expected: $100.25
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-100.25
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F31" authorId="0" shapeId="0">
       <text>
         <t>Expected: $70.06
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-70.06
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I31" authorId="0" shapeId="0">
       <text>
         <t>Expected: $425.50
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-425.50
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="J31" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,550.36
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-1,550.36
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="I32" authorId="0" shapeId="0">
       <text>
         <t>Expected: $244.05
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-244.05
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
       </text>
     </comment>
     <comment ref="F33" authorId="0" shapeId="0">
       <text>
         <t>Expected: $114.39
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-114.39
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
-      </text>
-    </comment>
-    <comment ref="F35" authorId="0" shapeId="0">
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0" shapeId="0">
       <text>
         <t>Expected: $306.45
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-306.45
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
-      </text>
-    </comment>
-    <comment ref="I35" authorId="0" shapeId="0">
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="I34" authorId="0" shapeId="0">
       <text>
         <t>Expected: $1,293.00
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-1,293.00
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
-      </text>
-    </comment>
-    <comment ref="J35" authorId="0" shapeId="0">
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="J34" authorId="0" shapeId="0">
       <text>
         <t>Expected: $2,969.96
-Found: $0.00
+Found in UNMATCHED transactions: $0.00
 Difference: $-2,969.96
-Transactions found: 0
-Reason: No transactions found for card type in date range</t>
+Unmatched transactions available: 0
+Note: 'Found' amount excludes transactions already matched elsewhere</t>
+      </text>
+    </comment>
+    <comment ref="B35" authorId="1" shapeId="0">
+      <text>
+        <t>Net Discrepancy:
+$461.14
+(Bank has ${abs(diff):,.2f} MORE than expected)
+Possible causes: duplicate transactions,
+unexpected charges, or misclassified items</t>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="1" shapeId="0">
+      <text>
+        <t>Net Discrepancy:
+$-942.34
+(Bank has ${abs(diff):,.2f} LESS than expected)
+Possible causes: missing transactions,
+unprocessed charges, or timing differences</t>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="1" shapeId="0">
+      <text>
+        <t>Net Discrepancy:
+$-2,700.87
+(Bank has ${abs(diff):,.2f} LESS than expected)
+Possible causes: missing transactions,
+unprocessed charges, or timing differences</t>
+      </text>
+    </comment>
+    <comment ref="I35" authorId="1" shapeId="0">
+      <text>
+        <t>Net Discrepancy:
+$-6,588.96
+(Bank has ${abs(diff):,.2f} LESS than expected)
+Possible causes: missing transactions,
+unprocessed charges, or timing differences</t>
+      </text>
+    </comment>
+    <comment ref="J35" authorId="1" shapeId="0">
+      <text>
+        <t>Net Discrepancy:
+$-12,689.95
+(Bank has ${abs(diff):,.2f} LESS than expected)
+Possible causes: missing transactions,
+unprocessed charges, or timing differences</t>
+      </text>
+    </comment>
+    <comment ref="K35" authorId="1" shapeId="0">
+      <text>
+        <t>Net Discrepancy:
+$60.92
+(Bank has ${abs(diff):,.2f} MORE than expected)
+Possible causes: duplicate transactions,
+unexpected charges, or misclassified items</t>
       </text>
     </comment>
   </commentList>
@@ -1292,7 +1404,7 @@
       <c r="E12" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="15" t="n">
         <v>-143.36</v>
       </c>
       <c r="G12" s="4" t="n">
@@ -1330,7 +1442,7 @@
       <c r="E13" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="15" t="n">
         <v>-38.76</v>
       </c>
       <c r="G13" s="14" t="n">
@@ -1406,7 +1518,7 @@
       <c r="E15" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="15" t="n">
         <v>-291.63</v>
       </c>
       <c r="G15" s="4" t="n">
@@ -1748,7 +1860,7 @@
       <c r="E24" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="15" t="n">
         <v>-136.36</v>
       </c>
       <c r="G24" s="14" t="n">
@@ -1763,7 +1875,7 @@
       <c r="J24" s="15" t="n">
         <v>4699.67</v>
       </c>
-      <c r="K24" s="4" t="n">
+      <c r="K24" s="15" t="n">
         <v>-60.92</v>
       </c>
       <c r="L24" s="4" t="n">
@@ -1786,7 +1898,7 @@
       <c r="E25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="15" t="n">
         <v>-341.71</v>
       </c>
       <c r="G25" s="4" t="n">
@@ -1888,7 +2000,7 @@
       <c r="A28" s="3" t="n">
         <v>45832</v>
       </c>
-      <c r="B28" s="4" t="n">
+      <c r="B28" s="14" t="n">
         <v>-105.75</v>
       </c>
       <c r="C28" s="14" t="n">
@@ -1900,7 +2012,7 @@
       <c r="E28" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="15" t="n">
         <v>-43.17</v>
       </c>
       <c r="G28" s="14" t="n">
@@ -2116,10 +2228,10 @@
       <c r="A34" s="3" t="n">
         <v>45838</v>
       </c>
-      <c r="B34" s="4" t="n">
+      <c r="B34" s="14" t="n">
         <v>10766.15</v>
       </c>
-      <c r="C34" s="4" t="n">
+      <c r="C34" s="14" t="n">
         <v>2546.49</v>
       </c>
       <c r="D34" s="5" t="n">
@@ -2128,22 +2240,22 @@
       <c r="E34" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="15" t="n">
         <v>306.45</v>
       </c>
-      <c r="G34" s="4" t="n">
+      <c r="G34" s="14" t="n">
         <v>362.72</v>
       </c>
       <c r="H34" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I34" s="4" t="n">
+      <c r="I34" s="15" t="n">
         <v>1293</v>
       </c>
-      <c r="J34" s="4" t="n">
+      <c r="J34" s="15" t="n">
         <v>2969.96</v>
       </c>
-      <c r="K34" s="4" t="n">
+      <c r="K34" s="14" t="n">
         <v>1337.8</v>
       </c>
       <c r="L34" s="4" t="n">
@@ -2156,10 +2268,10 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="B35" s="16" t="n">
+      <c r="B35" s="6" t="n">
         <v>373800.47</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="6" t="n">
         <v>103465.3</v>
       </c>
       <c r="D35" s="6" t="n">
@@ -2168,22 +2280,22 @@
       <c r="E35" s="6" t="n">
         <v>942.34</v>
       </c>
-      <c r="F35" s="17" t="n">
+      <c r="F35" s="6" t="n">
         <v>85497.02</v>
       </c>
-      <c r="G35" s="16" t="n">
+      <c r="G35" s="6" t="n">
         <v>30291.52</v>
       </c>
       <c r="H35" s="6" t="n">
         <v>2737.97</v>
       </c>
-      <c r="I35" s="17" t="n">
+      <c r="I35" s="6" t="n">
         <v>902.75</v>
       </c>
-      <c r="J35" s="17" t="n">
+      <c r="J35" s="6" t="n">
         <v>2881.96</v>
       </c>
-      <c r="K35" s="16" t="n">
+      <c r="K35" s="6" t="n">
         <v>25999.24</v>
       </c>
       <c r="L35" s="6" t="n">

</xml_diff>